<commit_message>
Update from construct mapping
</commit_message>
<xml_diff>
--- a/ModeOfDelivery/bcio_mode_of_delivery.xlsx
+++ b/ModeOfDelivery/bcio_mode_of_delivery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisazhang/Documents/GitHub/ontologies/ModeOfDelivery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D269D8-843E-4346-8E52-22DFD5138F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DF9E6D-581D-EA40-9339-38C3A848BD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="330">
   <si>
     <t>ID</t>
   </si>
@@ -986,13 +986,37 @@
   </si>
   <si>
     <t>BCI attribute</t>
+  </si>
+  <si>
+    <t>mass media mode of delivery</t>
+  </si>
+  <si>
+    <t>This is a form of mass media.</t>
+  </si>
+  <si>
+    <t>Informational mode of delivery of radio broadcast, television, online press and printed press to a mass audience.</t>
+  </si>
+  <si>
+    <t>online press mode of delivery</t>
+  </si>
+  <si>
+    <t>Electronic mode of delivery of a newspaper or magazine.</t>
+  </si>
+  <si>
+    <t>social influence intervention through mass media</t>
+  </si>
+  <si>
+    <t>A behaviour change intervention that is an awareness of other people’s thoughts, feelings and actions BCT delivered through a mass media mode of delivery.</t>
+  </si>
+  <si>
+    <t>behaviour change intervention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1029,12 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1338,13 +1368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="V58" sqref="V58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2921,21 +2954,17 @@
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>188</v>
-      </c>
+      <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>189</v>
+        <v>322</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>190</v>
+        <v>324</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>27</v>
@@ -2947,7 +2976,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>192</v>
+        <v>323</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2966,20 +2995,20 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>27</v>
@@ -2988,11 +3017,11 @@
         <v>28</v>
       </c>
       <c r="I38" s="2"/>
-      <c r="J38" s="2" t="s">
-        <v>197</v>
-      </c>
+      <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
+      <c r="L38" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2" t="s">
@@ -3010,17 +3039,17 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>26</v>
@@ -3032,7 +3061,9 @@
         <v>28</v>
       </c>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
@@ -3052,22 +3083,20 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>205</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>27</v>
@@ -3095,21 +3124,17 @@
       <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>207</v>
-      </c>
+      <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>208</v>
+        <v>325</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>209</v>
+        <v>326</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>27</v>
@@ -3120,9 +3145,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="2" t="s">
-        <v>211</v>
-      </c>
+      <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2" t="s">
@@ -3140,20 +3163,22 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D42" s="2"/>
+        <v>204</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="E42" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>27</v>
@@ -3182,20 +3207,20 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>27</v>
@@ -3206,7 +3231,9 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
+      <c r="L43" s="2" t="s">
+        <v>211</v>
+      </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2" t="s">
@@ -3224,20 +3251,20 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>220</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>27</v>
@@ -3248,9 +3275,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2" t="s">
-        <v>223</v>
-      </c>
+      <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2" t="s">
@@ -3268,20 +3293,20 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>27</v>
@@ -3292,9 +3317,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2" t="s">
-        <v>227</v>
-      </c>
+      <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2" t="s">
@@ -3312,20 +3335,20 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>178</v>
+        <v>26</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>27</v>
@@ -3337,12 +3360,10 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="M46" s="2"/>
-      <c r="N46" s="2" t="s">
-        <v>233</v>
-      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2" t="s">
         <v>30</v>
       </c>
@@ -3358,20 +3379,20 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>27</v>
@@ -3382,7 +3403,9 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2" t="s">
@@ -3400,22 +3423,20 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>241</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>27</v>
@@ -3426,9 +3447,13 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="L48" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+      <c r="N48" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="O48" s="2" t="s">
         <v>30</v>
       </c>
@@ -3444,22 +3469,20 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>239</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>41</v>
+        <v>178</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>27</v>
@@ -3488,20 +3511,22 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D50" s="2"/>
+        <v>240</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="E50" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>27</v>
@@ -3512,9 +3537,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="L50" s="2" t="s">
-        <v>250</v>
-      </c>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2" t="s">
@@ -3532,17 +3555,19 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D51" s="2"/>
+        <v>244</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="E51" s="2" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>41</v>
@@ -3556,9 +3581,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="L51" s="2" t="s">
-        <v>255</v>
-      </c>
+      <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2" t="s">
@@ -3576,20 +3599,20 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>27</v>
@@ -3598,11 +3621,11 @@
         <v>28</v>
       </c>
       <c r="I52" s="2"/>
-      <c r="J52" s="2" t="s">
-        <v>259</v>
-      </c>
+      <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="L52" s="2" t="s">
+        <v>250</v>
+      </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2" t="s">
@@ -3619,21 +3642,17 @@
       <c r="V52" s="2"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>260</v>
-      </c>
+      <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>261</v>
+        <v>327</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>262</v>
+        <v>328</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="2" t="s">
-        <v>263</v>
-      </c>
+      <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>158</v>
+        <v>329</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>27</v>
@@ -3662,19 +3681,17 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>46</v>
+        <v>252</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>41</v>
@@ -3688,7 +3705,9 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2" t="s">
+        <v>255</v>
+      </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2" t="s">
@@ -3706,20 +3725,20 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>268</v>
+        <v>81</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>27</v>
@@ -3728,11 +3747,11 @@
         <v>28</v>
       </c>
       <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="J55" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="K55" s="2"/>
-      <c r="L55" s="2" t="s">
-        <v>271</v>
-      </c>
+      <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2" t="s">
@@ -3750,20 +3769,20 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>27</v>
@@ -3792,20 +3811,22 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>277</v>
+        <v>46</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D57" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E57" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>27</v>
@@ -3834,20 +3855,20 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>27</v>
@@ -3858,7 +3879,9 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
+      <c r="L58" s="2" t="s">
+        <v>271</v>
+      </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" s="2" t="s">
@@ -3876,22 +3899,20 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>27</v>
@@ -3920,20 +3941,20 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>27</v>
@@ -3962,20 +3983,20 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>27</v>
@@ -4004,20 +4025,22 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>296</v>
+        <v>164</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D62" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="E62" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>27</v>
@@ -4046,20 +4069,20 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>27</v>
@@ -4088,17 +4111,17 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>26</v>
@@ -4112,9 +4135,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-      <c r="L64" s="2" t="s">
-        <v>307</v>
-      </c>
+      <c r="L64" s="2"/>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2" t="s">
@@ -4132,20 +4153,20 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>27</v>
@@ -4156,9 +4177,7 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
-      <c r="L65" s="2" t="s">
-        <v>312</v>
-      </c>
+      <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2" t="s">
@@ -4176,20 +4195,20 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>27</v>
@@ -4218,17 +4237,17 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>26</v>
@@ -4242,7 +4261,9 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
+      <c r="L67" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2" t="s">
@@ -4258,7 +4279,136 @@
       </c>
       <c r="V67" s="2"/>
     </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V68" s="2"/>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V69" s="2"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2"/>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V70" s="2"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>